<commit_message>
Copied Latest Design in Folder  \Latest PCB Design
</commit_message>
<xml_diff>
--- a/BOMs/Lid Board May21.xlsx
+++ b/BOMs/Lid Board May21.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://teamairzai-my.sharepoint.com/personal/kashif_airzai_com/Documents/Airzai/GitHub/Airzai-Hardware/BOMs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kashif\OneDrive - Airzai\Airzai\GitHub\Airzai-Hardware\BOMs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{60998CE9-1464-4F3C-9810-1092092E4A63}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="8_{60998CE9-1464-4F3C-9810-1092092E4A63}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{9F528B04-228B-48E5-8467-0D1EFADEE90C}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="30915" windowHeight="15796" xr2:uid="{E294DC3A-9D89-4200-8E6A-ADE5D2CE6F9C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E294DC3A-9D89-4200-8E6A-ADE5D2CE6F9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="117">
   <si>
     <t>Reference Designator</t>
   </si>
@@ -339,9 +339,6 @@
     <t/>
   </si>
   <si>
-    <t>SKRAAKE010</t>
-  </si>
-  <si>
     <t>T1</t>
   </si>
   <si>
@@ -373,13 +370,25 @@
   </si>
   <si>
     <t>ACCEL 2-16G I2C/SPI 14LGA</t>
+  </si>
+  <si>
+    <t>Power inductor, dual-wound, 20% tol, SMT</t>
+  </si>
+  <si>
+    <t>CoilCraft</t>
+  </si>
+  <si>
+    <t>EVQ-QXM03W</t>
+  </si>
+  <si>
+    <t>SWITCH TACTILE SPST-NO 0.02A 15V</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -392,6 +401,13 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -414,10 +430,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -732,15 +749,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9046E1D8-5422-41CB-9B34-1FA6442CD430}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -760,7 +787,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -780,7 +807,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -800,7 +827,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -820,7 +847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -840,7 +867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
@@ -860,7 +887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>29</v>
       </c>
@@ -880,7 +907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>33</v>
       </c>
@@ -900,7 +927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>37</v>
       </c>
@@ -920,7 +947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>42</v>
       </c>
@@ -940,7 +967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>47</v>
       </c>
@@ -960,7 +987,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>52</v>
       </c>
@@ -980,7 +1007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>56</v>
       </c>
@@ -1000,7 +1027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>61</v>
       </c>
@@ -1020,7 +1047,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>66</v>
       </c>
@@ -1040,7 +1067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>71</v>
       </c>
@@ -1060,7 +1087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>75</v>
       </c>
@@ -1080,7 +1107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>79</v>
       </c>
@@ -1100,7 +1127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>83</v>
       </c>
@@ -1120,7 +1147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>87</v>
       </c>
@@ -1140,7 +1167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>91</v>
       </c>
@@ -1160,7 +1187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>96</v>
       </c>
@@ -1180,81 +1207,81 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>100</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>101</v>
+        <v>62</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E23" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>101</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+        <v>113</v>
+      </c>
+      <c r="F24" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="F25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="F25" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A26" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>113</v>
       </c>
       <c r="F26" s="2">
         <v>1</v>
@@ -1262,5 +1289,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="86" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>